<commit_message>
Updated Results Email Automation
</commit_message>
<xml_diff>
--- a/FlipkartExercise.xlsx
+++ b/FlipkartExercise.xlsx
@@ -181,8 +181,47 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="52">
+  <x:cellStyleXfs count="65">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>

</xml_diff>